<commit_message>
Added bottom pour GND Added thermal relieves for through holes Changed the RGB led GPIOs in order to have PWM Updated BOM Moved to version v1.2
</commit_message>
<xml_diff>
--- a/IRIS2/01-Design/IRIS2_PCB_CPU/Project Outputs for IRIS2_PCB_CPU/20210401_IRIS2_PCB_CPU_BOM.xlsx
+++ b/IRIS2/01-Design/IRIS2_PCB_CPU/Project Outputs for IRIS2_PCB_CPU/20210401_IRIS2_PCB_CPU_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bultz\workspace_daedalus\IRIS2\IRIS2\01-Design\IRIS2_PCB_CPU\Project Outputs for IRIS2_PCB_CPU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2322C580-434D-4FBE-BF44-795B6A133E06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5BEBD3-21CD-448D-85E1-F8D690B0A203}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{DBB1DBBE-08D7-45E2-8223-98B23C343DDE}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">IRIS2_PCB_CPU_BOM!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="131">
   <si>
     <t>Designator</t>
   </si>
@@ -249,12 +249,6 @@
     <t>Texas Instruments</t>
   </si>
   <si>
-    <t>MSP430FR5994</t>
-  </si>
-  <si>
-    <t>MSP430FR59941PN</t>
-  </si>
-  <si>
     <t>U2</t>
   </si>
   <si>
@@ -280,12 +274,6 @@
   </si>
   <si>
     <t>U5</t>
-  </si>
-  <si>
-    <t>TMP175C-Q1</t>
-  </si>
-  <si>
-    <t>TMP75C-Q1</t>
   </si>
   <si>
     <t>U6</t>
@@ -425,6 +413,24 @@
   </si>
   <si>
     <t>THD</t>
+  </si>
+  <si>
+    <t>MSP430FR5994IPNR</t>
+  </si>
+  <si>
+    <t>MSP430FR5994IPN</t>
+  </si>
+  <si>
+    <t>INA226AQDGSRQ1</t>
+  </si>
+  <si>
+    <t>MS561101BA03-50</t>
+  </si>
+  <si>
+    <t>TMP175AIDR</t>
+  </si>
+  <si>
+    <t>TMP75C-Q1 SOIC</t>
   </si>
 </sst>
 </file>
@@ -833,7 +839,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,7 +869,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>5</v>
@@ -886,10 +892,10 @@
         <v>9</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -909,10 +915,10 @@
         <v>12</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -932,10 +938,10 @@
         <v>15</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -955,10 +961,10 @@
         <v>19</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -978,10 +984,10 @@
         <v>12</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1001,10 +1007,10 @@
         <v>9</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1024,10 +1030,10 @@
         <v>9</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1047,10 +1053,10 @@
         <v>28</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1070,10 +1076,10 @@
         <v>32</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1093,10 +1099,10 @@
         <v>35</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1116,10 +1122,10 @@
         <v>39</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1139,10 +1145,10 @@
         <v>41</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1162,10 +1168,10 @@
         <v>43</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1185,10 +1191,10 @@
         <v>46</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1208,10 +1214,10 @@
         <v>49</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1231,10 +1237,10 @@
         <v>9</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1254,10 +1260,10 @@
         <v>9</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1277,10 +1283,10 @@
         <v>9</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1300,10 +1306,10 @@
         <v>9</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1323,10 +1329,10 @@
         <v>61</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1346,10 +1352,10 @@
         <v>9</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1369,10 +1375,10 @@
         <v>67</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1386,21 +1392,21 @@
         <v>69</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>70</v>
+        <v>125</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>71</v>
+        <v>126</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B25" s="4">
         <v>1</v>
@@ -1409,67 +1415,67 @@
         <v>69</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>73</v>
+        <v>127</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" s="4">
+        <v>1</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="4">
-        <v>1</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="F26" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" s="4">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B27" s="4">
-        <v>1</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>79</v>
-      </c>
       <c r="E27" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B28" s="4">
         <v>1</v>
@@ -1478,67 +1484,67 @@
         <v>69</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>81</v>
+        <v>129</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>82</v>
+        <v>130</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B29" s="4">
         <v>1</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B30" s="4">
         <v>1</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B31" s="4">
         <v>4</v>
@@ -1547,21 +1553,21 @@
         <v>69</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B32" s="4">
         <v>1</v>
@@ -1570,62 +1576,62 @@
         <v>30</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B33" s="4">
         <v>1</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B34" s="4">
         <v>2</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>